<commit_message>
Add real Koenig Solutions team directory with 15 employees
</commit_message>
<xml_diff>
--- a/data/Team_Directory.xlsx
+++ b/data/Team_Directory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Employee_ID</t>
   </si>
@@ -31,82 +31,169 @@
     <t>Type</t>
   </si>
   <si>
-    <t>EMP001</t>
-  </si>
-  <si>
-    <t>EMP002</t>
-  </si>
-  <si>
-    <t>EMP003</t>
+    <t>EMP1086</t>
+  </si>
+  <si>
+    <t>EMP3638</t>
+  </si>
+  <si>
+    <t>EMP2627</t>
+  </si>
+  <si>
+    <t>EMP3411</t>
+  </si>
+  <si>
+    <t>EMP3412</t>
+  </si>
+  <si>
+    <t>EMP521</t>
+  </si>
+  <si>
+    <t>EMP2411</t>
+  </si>
+  <si>
+    <t>EMP3306</t>
+  </si>
+  <si>
+    <t>EMP2211</t>
+  </si>
+  <si>
+    <t>EMP004</t>
+  </si>
+  <si>
+    <t>EMP3201</t>
+  </si>
+  <si>
+    <t>EMP3313</t>
+  </si>
+  <si>
+    <t>EMP3135</t>
+  </si>
+  <si>
+    <t>EMP2979</t>
+  </si>
+  <si>
+    <t>EMP1687</t>
   </si>
   <si>
     <t>DEPT-HR</t>
   </si>
   <si>
-    <t>DEPT-TAX</t>
-  </si>
-  <si>
-    <t>DEPT-FIN</t>
-  </si>
-  <si>
-    <t>DEPT-ACC</t>
-  </si>
-  <si>
-    <t>Aditya Kumar</t>
-  </si>
-  <si>
-    <t>Anurag Sharma</t>
-  </si>
-  <si>
-    <t>Praveen Chaudhary</t>
-  </si>
-  <si>
-    <t>HR Department</t>
-  </si>
-  <si>
-    <t>Tax Department</t>
-  </si>
-  <si>
-    <t>Finance Team</t>
-  </si>
-  <si>
-    <t>Accounts Team</t>
-  </si>
-  <si>
-    <t>aditya@koenig-solutions.com</t>
-  </si>
-  <si>
-    <t>anurag@koenig-solutions.com</t>
+    <t>DEPT-AP</t>
+  </si>
+  <si>
+    <t>DEPT-AR</t>
+  </si>
+  <si>
+    <t>Sunil Kushwaha</t>
+  </si>
+  <si>
+    <t>Sarika Gupta</t>
+  </si>
+  <si>
+    <t>Ritika Bhalla</t>
+  </si>
+  <si>
+    <t>Tripti Sharma</t>
+  </si>
+  <si>
+    <t>Jony Saini</t>
+  </si>
+  <si>
+    <t>Anurag Chauhan</t>
+  </si>
+  <si>
+    <t>Ajay Rawat</t>
+  </si>
+  <si>
+    <t>Aditya Singh</t>
+  </si>
+  <si>
+    <t>Jatin Khurana</t>
+  </si>
+  <si>
+    <t>Praveen Kumar</t>
+  </si>
+  <si>
+    <t>Vipin Nautiyal</t>
+  </si>
+  <si>
+    <t>Tamanna Alisha</t>
+  </si>
+  <si>
+    <t>Nishant Yash</t>
+  </si>
+  <si>
+    <t>Shkelzen Sadiku</t>
+  </si>
+  <si>
+    <t>Nupur Munjal</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Accounts Payable</t>
+  </si>
+  <si>
+    <t>Accounts Receivable</t>
+  </si>
+  <si>
+    <t>Sunilkumar.kushwaha@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>sarika.gupta@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>ritika.bhalla@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>tripti@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>jony.saini@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>anurag.chauhan@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>ajay.rawat@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>aditya.singh@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>jatin.khurana@koenig-solutions.com</t>
   </si>
   <si>
     <t>praveen.chaudhary@koenig-solutions.com</t>
   </si>
   <si>
-    <t>hr@koenig-solutions.com</t>
-  </si>
-  <si>
-    <t>tax@koenig-solutions.com</t>
-  </si>
-  <si>
-    <t>finance@koenig-solutions.com</t>
-  </si>
-  <si>
-    <t>accounts@koenig-solutions.com</t>
+    <t>vipin.nautiyal@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>tamanna.alisha@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>nishant.yash@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>Shkelzen.Sadiku@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>nupur.munjal@koenig-solutions.com</t>
+  </si>
+  <si>
+    <t>A&amp;F</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>COM EA Team</t>
   </si>
   <si>
     <t>Finance</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Accounts</t>
   </si>
   <si>
     <t>Individual</t>
@@ -467,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,16 +582,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -512,16 +599,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -529,16 +616,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -546,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -563,16 +650,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -580,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -597,15 +684,202 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update entire project with smart reply automation
</commit_message>
<xml_diff>
--- a/data/Team_Directory.xlsx
+++ b/data/Team_Directory.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/praveenchaudhary/Downloads/Agent/followup-reminder-agent/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E864E5-EB7C-9542-8D01-5189A6C56BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -202,8 +208,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +272,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +324,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -344,6 +358,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -378,9 +393,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,14 +569,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -594,7 +612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -611,7 +629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -628,7 +646,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -645,7 +663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -662,7 +680,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -679,7 +697,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -696,7 +714,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -713,7 +731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -730,7 +748,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -747,7 +765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -764,7 +782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -781,7 +799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -798,7 +816,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -815,7 +833,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -832,7 +850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -849,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -866,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>

</xml_diff>